<commit_message>
元神需求 3 6 9 10 12 13 品
</commit_message>
<xml_diff>
--- a/src/main/resources/CardPiece.xlsx
+++ b/src/main/resources/CardPiece.xlsx
@@ -7,7 +7,13 @@
     <workbookView windowWidth="23895" windowHeight="10500"/>
   </bookViews>
   <sheets>
-    <sheet name="14" sheetId="1" r:id="rId1"/>
+    <sheet name="3" sheetId="2" r:id="rId1"/>
+    <sheet name="6" sheetId="3" r:id="rId2"/>
+    <sheet name="9" sheetId="4" r:id="rId3"/>
+    <sheet name="10" sheetId="5" r:id="rId4"/>
+    <sheet name="12" sheetId="6" r:id="rId5"/>
+    <sheet name="13" sheetId="7" r:id="rId6"/>
+    <sheet name="14" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -17,6 +23,9 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16">
   <si>
     <t>聚魂</t>
+  </si>
+  <si>
+    <t>合计</t>
   </si>
   <si>
     <t>修炼</t>
@@ -60,9 +69,6 @@
   <si>
     <t>云裳</t>
   </si>
-  <si>
-    <t>合计</t>
-  </si>
 </sst>
 </file>
 
@@ -70,9 +76,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -80,6 +86,52 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -91,7 +143,38 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -112,34 +195,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -152,37 +212,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -197,31 +227,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -236,187 +242,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -427,15 +433,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -454,16 +451,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -502,16 +499,25 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -535,10 +541,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -547,133 +553,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1003,9 +1009,354 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="2:2">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <f>SUM(B2:B2)</f>
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="2:2">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <f>SUM(B2:B2)</f>
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="7" outlineLevelCol="2"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="2:3">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <f>SUM(B2:B7)</f>
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <f>SUM(C2:C7)</f>
+        <v>250</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="7" outlineLevelCol="2"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="2:3">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <f>SUM(B2:B7)</f>
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <f>SUM(C2:C7)</f>
+        <v>250</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="7" outlineLevelCol="2"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="2:3">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <f>SUM(B2:B7)</f>
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <f>SUM(C2:C7)</f>
+        <v>250</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1016,46 +1367,46 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -1271,7 +1622,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1296,8 +1647,14 @@
       <c r="L8">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="N8">
+        <v>80</v>
+      </c>
+      <c r="O8">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1319,8 +1676,14 @@
       <c r="L9">
         <v>75</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="N9">
+        <v>80</v>
+      </c>
+      <c r="O9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1342,8 +1705,14 @@
       <c r="L10">
         <v>90</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="N10">
+        <v>80</v>
+      </c>
+      <c r="O10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1364,6 +1733,12 @@
       </c>
       <c r="L11">
         <v>120</v>
+      </c>
+      <c r="N11">
+        <v>80</v>
+      </c>
+      <c r="O11">
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1608,7 +1983,7 @@
     </row>
     <row r="42" spans="1:16">
       <c r="A42" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B42">
         <f t="shared" ref="B42:P42" si="0">SUM(B2:B41)</f>
@@ -1660,11 +2035,712 @@
       </c>
       <c r="N42">
         <f t="shared" si="0"/>
-        <v>276</v>
+        <v>596</v>
       </c>
       <c r="O42">
         <f t="shared" si="0"/>
-        <v>276</v>
+        <v>596</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:P42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="2:16">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>40</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>40</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>40</v>
+      </c>
+      <c r="K2">
+        <v>40</v>
+      </c>
+      <c r="L2">
+        <v>6</v>
+      </c>
+      <c r="M2">
+        <v>60</v>
+      </c>
+      <c r="N2">
+        <v>16</v>
+      </c>
+      <c r="O2">
+        <v>16</v>
+      </c>
+      <c r="P2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>8</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="L3">
+        <v>12</v>
+      </c>
+      <c r="N3">
+        <v>24</v>
+      </c>
+      <c r="O3">
+        <v>24</v>
+      </c>
+      <c r="P3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>20</v>
+      </c>
+      <c r="H4">
+        <v>12</v>
+      </c>
+      <c r="I4">
+        <v>20</v>
+      </c>
+      <c r="L4">
+        <v>18</v>
+      </c>
+      <c r="N4">
+        <v>32</v>
+      </c>
+      <c r="O4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>40</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>30</v>
+      </c>
+      <c r="H5">
+        <v>16</v>
+      </c>
+      <c r="I5">
+        <v>30</v>
+      </c>
+      <c r="L5">
+        <v>24</v>
+      </c>
+      <c r="N5">
+        <v>52</v>
+      </c>
+      <c r="O5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>80</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>40</v>
+      </c>
+      <c r="H6">
+        <v>20</v>
+      </c>
+      <c r="I6">
+        <v>40</v>
+      </c>
+      <c r="L6">
+        <v>30</v>
+      </c>
+      <c r="N6">
+        <v>72</v>
+      </c>
+      <c r="O6">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>120</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>15</v>
+      </c>
+      <c r="G7">
+        <v>60</v>
+      </c>
+      <c r="H7">
+        <v>30</v>
+      </c>
+      <c r="I7">
+        <v>60</v>
+      </c>
+      <c r="L7">
+        <v>45</v>
+      </c>
+      <c r="N7">
+        <v>80</v>
+      </c>
+      <c r="O7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>160</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>20</v>
+      </c>
+      <c r="G8">
+        <v>80</v>
+      </c>
+      <c r="H8">
+        <v>40</v>
+      </c>
+      <c r="I8">
+        <v>80</v>
+      </c>
+      <c r="L8">
+        <v>60</v>
+      </c>
+      <c r="N8">
+        <v>80</v>
+      </c>
+      <c r="O8">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>25</v>
+      </c>
+      <c r="G9">
+        <v>100</v>
+      </c>
+      <c r="H9">
+        <v>50</v>
+      </c>
+      <c r="I9">
+        <v>100</v>
+      </c>
+      <c r="L9">
+        <v>75</v>
+      </c>
+      <c r="N9">
+        <v>80</v>
+      </c>
+      <c r="O9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>30</v>
+      </c>
+      <c r="G10">
+        <v>120</v>
+      </c>
+      <c r="H10">
+        <v>60</v>
+      </c>
+      <c r="I10">
+        <v>120</v>
+      </c>
+      <c r="L10">
+        <v>90</v>
+      </c>
+      <c r="N10">
+        <v>80</v>
+      </c>
+      <c r="O10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="F11">
+        <v>40</v>
+      </c>
+      <c r="G11">
+        <v>160</v>
+      </c>
+      <c r="H11">
+        <v>80</v>
+      </c>
+      <c r="I11">
+        <v>160</v>
+      </c>
+      <c r="L11">
+        <v>120</v>
+      </c>
+      <c r="N11">
+        <v>80</v>
+      </c>
+      <c r="O11">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="D16">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="D26">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="D27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="D29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="D30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="D31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="D32">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="D33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="D34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="D35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="D36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="D37">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="D38">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="D39">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="D40">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="D41">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
+      <c r="A42" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42">
+        <f t="shared" ref="B42:P42" si="0">SUM(B2:B41)</f>
+        <v>40</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>410</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>370</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="0"/>
+        <v>625</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="0"/>
+        <v>320</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="0"/>
+        <v>625</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="0"/>
+        <v>480</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="0"/>
+        <v>596</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="0"/>
+        <v>596</v>
       </c>
       <c r="P42">
         <f t="shared" si="0"/>

</xml_diff>